<commit_message>
Generate plots and stats
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlfre\OneDrive\Documents\__my_files\01-repos\public\crispr-ga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B50C19B-3A0B-4018-A0F5-E7923EF431DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D5905A-FC62-451E-A097-3359FC253151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{453CAC28-61B3-4AC6-B2DB-3F6E75A82C77}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{453CAC28-61B3-4AC6-B2DB-3F6E75A82C77}"/>
   </bookViews>
   <sheets>
     <sheet name="0.10" sheetId="1" r:id="rId1"/>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC221F10-870C-4869-B091-338AA4ED287E}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Y29"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,94 +847,434 @@
         <v>530562.02526763</v>
       </c>
     </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>424994.22190781898</v>
+      </c>
+      <c r="C7">
+        <v>373216.479737752</v>
+      </c>
+      <c r="D7">
+        <v>553646.17735026404</v>
+      </c>
+      <c r="E7">
+        <v>663630.38074962201</v>
+      </c>
+      <c r="F7">
+        <v>649296.51776430197</v>
+      </c>
+      <c r="G7">
+        <v>848138.26708517701</v>
+      </c>
+      <c r="H7">
+        <v>1448680.45223067</v>
+      </c>
+      <c r="I7">
+        <v>917968.25825960399</v>
+      </c>
+      <c r="J7">
+        <v>1713406.3151701801</v>
+      </c>
+      <c r="K7">
+        <v>6042153.9761082996</v>
+      </c>
+      <c r="L7">
+        <v>14621671.684563201</v>
+      </c>
+      <c r="O7">
+        <v>11015.0239113718</v>
+      </c>
+      <c r="P7">
+        <v>20791.9131442904</v>
+      </c>
+      <c r="Q7">
+        <v>19569.887382909601</v>
+      </c>
+      <c r="R7">
+        <v>24433.4779717028</v>
+      </c>
+      <c r="S7">
+        <v>22222.119554877201</v>
+      </c>
+      <c r="T7">
+        <v>26028.685137629502</v>
+      </c>
+      <c r="U7">
+        <v>29526.020504534201</v>
+      </c>
+      <c r="V7">
+        <v>39379.541855305397</v>
+      </c>
+      <c r="W7">
+        <v>72845.273867249402</v>
+      </c>
+      <c r="X7">
+        <v>180939.75542485699</v>
+      </c>
+      <c r="Y7">
+        <v>559409.67557765497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>424748.18781187001</v>
+      </c>
+      <c r="C8">
+        <v>427575.34951368801</v>
+      </c>
+      <c r="D8">
+        <v>548830.69392687595</v>
+      </c>
+      <c r="E8">
+        <v>670062.56436329102</v>
+      </c>
+      <c r="F8">
+        <v>643933.26588632702</v>
+      </c>
+      <c r="G8">
+        <v>853208.06684915302</v>
+      </c>
+      <c r="H8">
+        <v>1385288.1292256</v>
+      </c>
+      <c r="I8">
+        <v>936228.82282138604</v>
+      </c>
+      <c r="J8">
+        <v>1694053.3844773199</v>
+      </c>
+      <c r="K8">
+        <v>6056190.50548869</v>
+      </c>
+      <c r="L8">
+        <v>14640138.884045901</v>
+      </c>
+      <c r="O8">
+        <v>11579.7726418823</v>
+      </c>
+      <c r="P8">
+        <v>19159.459115937301</v>
+      </c>
+      <c r="Q8">
+        <v>20122.922617942</v>
+      </c>
+      <c r="R8">
+        <v>21321.060145273801</v>
+      </c>
+      <c r="S8">
+        <v>20517.7532173693</v>
+      </c>
+      <c r="T8">
+        <v>23763.917727395801</v>
+      </c>
+      <c r="U8">
+        <v>39186.260439455502</v>
+      </c>
+      <c r="V8">
+        <v>43750.6276667118</v>
+      </c>
+      <c r="W8">
+        <v>76132.871767506003</v>
+      </c>
+      <c r="X8">
+        <v>166978.42688113399</v>
+      </c>
+      <c r="Y8">
+        <v>596200.33151470101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>422838.45179500902</v>
+      </c>
+      <c r="C9">
+        <v>415063.38948454498</v>
+      </c>
+      <c r="D9">
+        <v>555897.92507237894</v>
+      </c>
+      <c r="E9">
+        <v>670939.34679340699</v>
+      </c>
+      <c r="F9">
+        <v>642802.44953961996</v>
+      </c>
+      <c r="G9">
+        <v>864060.09580281004</v>
+      </c>
+      <c r="H9">
+        <v>1458620.20081292</v>
+      </c>
+      <c r="I9">
+        <v>930575.12784951401</v>
+      </c>
+      <c r="J9">
+        <v>1693101.7454067001</v>
+      </c>
+      <c r="K9">
+        <v>6007260.4570507696</v>
+      </c>
+      <c r="L9">
+        <v>14607634.595560201</v>
+      </c>
+      <c r="O9">
+        <v>13017.9940089583</v>
+      </c>
+      <c r="P9">
+        <v>22304.0826264768</v>
+      </c>
+      <c r="Q9">
+        <v>22075.7972449064</v>
+      </c>
+      <c r="R9">
+        <v>22728.470731526599</v>
+      </c>
+      <c r="S9">
+        <v>23600.9952649474</v>
+      </c>
+      <c r="T9">
+        <v>20735.4797888547</v>
+      </c>
+      <c r="U9">
+        <v>36941.396327689203</v>
+      </c>
+      <c r="V9">
+        <v>41761.149210855299</v>
+      </c>
+      <c r="W9">
+        <v>73986.160583794102</v>
+      </c>
+      <c r="X9">
+        <v>202753.40924412</v>
+      </c>
+      <c r="Y9">
+        <v>505187.202041968</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>442335.63341076399</v>
+      </c>
+      <c r="C10">
+        <v>407592.37785540399</v>
+      </c>
+      <c r="D10">
+        <v>526028.57193360105</v>
+      </c>
+      <c r="E10">
+        <v>649241.04780065303</v>
+      </c>
+      <c r="F10">
+        <v>637162.18521806097</v>
+      </c>
+      <c r="G10">
+        <v>835091.55859278701</v>
+      </c>
+      <c r="H10">
+        <v>1427686.5546063799</v>
+      </c>
+      <c r="I10">
+        <v>917329.26830926305</v>
+      </c>
+      <c r="J10">
+        <v>1686294.8904053599</v>
+      </c>
+      <c r="K10">
+        <v>6039298.6351100001</v>
+      </c>
+      <c r="L10">
+        <v>14655590.1978737</v>
+      </c>
+      <c r="O10">
+        <v>10763.1358075886</v>
+      </c>
+      <c r="P10">
+        <v>17572.94925116</v>
+      </c>
+      <c r="Q10">
+        <v>17789.217315614202</v>
+      </c>
+      <c r="R10">
+        <v>22576.907206326701</v>
+      </c>
+      <c r="S10">
+        <v>31850.275343284</v>
+      </c>
+      <c r="T10">
+        <v>23608.458707108999</v>
+      </c>
+      <c r="U10">
+        <v>36106.131421402097</v>
+      </c>
+      <c r="V10">
+        <v>54325.599066913099</v>
+      </c>
+      <c r="W10">
+        <v>58372.318157926202</v>
+      </c>
+      <c r="X10">
+        <v>184548.2574068</v>
+      </c>
+      <c r="Y10">
+        <v>574256.10653124703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>430898.01976817899</v>
+      </c>
+      <c r="C11">
+        <v>398549.51780801802</v>
+      </c>
+      <c r="D11">
+        <v>534618.03308232501</v>
+      </c>
+      <c r="E11">
+        <v>658302.19824889803</v>
+      </c>
+      <c r="F11">
+        <v>655822.11513757904</v>
+      </c>
+      <c r="G11">
+        <v>856247.37213183998</v>
+      </c>
+      <c r="H11">
+        <v>1439675.08579146</v>
+      </c>
+      <c r="I11">
+        <v>890773.59113979305</v>
+      </c>
+      <c r="J11">
+        <v>1711915.13322142</v>
+      </c>
+      <c r="K11">
+        <v>5999357.2746209903</v>
+      </c>
+      <c r="L11">
+        <v>14651346.015616899</v>
+      </c>
+      <c r="O11">
+        <v>13441.3131717592</v>
+      </c>
+      <c r="P11">
+        <v>15634.484896436299</v>
+      </c>
+      <c r="Q11">
+        <v>19075.265921652299</v>
+      </c>
+      <c r="R11">
+        <v>24309.171071276</v>
+      </c>
+      <c r="S11">
+        <v>26080.841124057701</v>
+      </c>
+      <c r="T11">
+        <v>23263.130672275998</v>
+      </c>
+      <c r="U11">
+        <v>41612.482778728001</v>
+      </c>
+      <c r="V11">
+        <v>48734.386064112099</v>
+      </c>
+      <c r="W11">
+        <v>75153.234601020798</v>
+      </c>
+      <c r="X11">
+        <v>169167.135344818</v>
+      </c>
+      <c r="Y11">
+        <v>516557.05714039499</v>
+      </c>
+    </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>AVERAGE(B2:B11)</f>
-        <v>418749.47123797843</v>
+        <v>423956.18708835338</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:L12" si="0">AVERAGE(C2:C11)</f>
-        <v>411995.62237263261</v>
+        <v>408197.52262625692</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>534124.24901386118</v>
+        <v>538964.26464347506</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>659640.35046125564</v>
+        <v>661037.7290262148</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>653076.20368010562</v>
+        <v>649439.75519464177</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>846845.48499425896</v>
+        <v>849097.27854330617</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1429546.920879886</v>
+        <v>1430768.5027066458</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>927144.03836381657</v>
+        <v>922859.52601986437</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>1704117.3747880161</v>
+        <v>1701935.8342621061</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>6026636.2286063442</v>
+        <v>6027744.199141046</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>14613990.668556279</v>
+        <v>14624633.472044131</v>
       </c>
       <c r="O12">
         <f>AVERAGE(O2:O11)</f>
-        <v>11701.46919377142</v>
+        <v>11832.458551041729</v>
       </c>
       <c r="P12">
         <f t="shared" ref="P12" si="1">AVERAGE(P2:P11)</f>
-        <v>15566.429244726838</v>
+        <v>17329.503525793501</v>
       </c>
       <c r="Q12">
         <f t="shared" ref="Q12" si="2">AVERAGE(Q2:Q11)</f>
-        <v>17112.88837529712</v>
+        <v>18419.753235951008</v>
       </c>
       <c r="R12">
         <f t="shared" ref="R12" si="3">AVERAGE(R2:R11)</f>
-        <v>19216.441497579181</v>
+        <v>21145.129461400178</v>
       </c>
       <c r="S12">
         <f t="shared" ref="S12" si="4">AVERAGE(S2:S11)</f>
-        <v>20347.205872088642</v>
+        <v>22600.801386497878</v>
       </c>
       <c r="T12">
         <f t="shared" ref="T12" si="5">AVERAGE(T2:T11)</f>
-        <v>21764.159085601517</v>
+        <v>22622.046746127256</v>
       </c>
       <c r="U12">
         <f t="shared" ref="U12" si="6">AVERAGE(U2:U11)</f>
-        <v>31858.372814580758</v>
+        <v>34266.415554471278</v>
       </c>
       <c r="V12">
         <f t="shared" ref="V12" si="7">AVERAGE(V2:V11)</f>
-        <v>40179.343504458622</v>
+        <v>42884.802138619081</v>
       </c>
       <c r="W12">
         <f t="shared" ref="W12" si="8">AVERAGE(W2:W11)</f>
-        <v>72689.159478992195</v>
+        <v>71993.565637245745</v>
       </c>
       <c r="X12">
         <f t="shared" ref="X12" si="9">AVERAGE(X2:X11)</f>
-        <v>181690.74773825679</v>
+        <v>181284.07229930133</v>
       </c>
       <c r="Y12">
         <f t="shared" ref="Y12" si="10">AVERAGE(Y2:Y11)</f>
-        <v>524083.15863460238</v>
+        <v>537202.61659789772</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -975,47 +1315,47 @@
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>B12/B13</f>
-        <v>3.8716100485209592</v>
+        <v>3.9197495084861491</v>
       </c>
       <c r="C14">
         <f t="shared" ref="C14:L14" si="11">C12/C13</f>
-        <v>9.2994971530738919</v>
+        <v>9.2137670727999659</v>
       </c>
       <c r="D14">
         <f t="shared" si="11"/>
-        <v>9.0483525159048135</v>
+        <v>9.1303449880310872</v>
       </c>
       <c r="E14">
         <f t="shared" si="11"/>
-        <v>6.8164381273638615</v>
+        <v>6.8308780331729713</v>
       </c>
       <c r="F14">
         <f t="shared" si="11"/>
-        <v>11.156639453339009</v>
+        <v>11.094517231744739</v>
       </c>
       <c r="G14">
         <f t="shared" si="11"/>
-        <v>11.493247808070613</v>
+        <v>11.523808780208276</v>
       </c>
       <c r="H14">
         <f t="shared" si="11"/>
-        <v>17.787292623771428</v>
+        <v>17.80249228815396</v>
       </c>
       <c r="I14">
         <f t="shared" si="11"/>
-        <v>18.86932000333401</v>
+        <v>18.782121217459334</v>
       </c>
       <c r="J14">
         <f t="shared" si="11"/>
-        <v>15.894096783047614</v>
+        <v>15.873749818238769</v>
       </c>
       <c r="K14">
         <f t="shared" si="11"/>
-        <v>23.264823596696882</v>
+        <v>23.269100732077614</v>
       </c>
       <c r="L14">
         <f t="shared" si="11"/>
-        <v>38.658078333464573</v>
+        <v>38.686231514909139</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -1432,94 +1772,434 @@
         <v>436090.11541120702</v>
       </c>
     </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>449840.635895618</v>
+      </c>
+      <c r="C22">
+        <v>436579.48141684599</v>
+      </c>
+      <c r="D22">
+        <v>572395.26925963105</v>
+      </c>
+      <c r="E22">
+        <v>655472.62867309805</v>
+      </c>
+      <c r="F22">
+        <v>687500.90038117499</v>
+      </c>
+      <c r="G22">
+        <v>874438.33537245402</v>
+      </c>
+      <c r="H22">
+        <v>1452671.7333620901</v>
+      </c>
+      <c r="I22">
+        <v>948177.732654867</v>
+      </c>
+      <c r="J22">
+        <v>1722605.26161585</v>
+      </c>
+      <c r="K22">
+        <v>6007004.0678088497</v>
+      </c>
+      <c r="L22">
+        <v>14588930.785886999</v>
+      </c>
+      <c r="O22">
+        <v>8829.8604488372803</v>
+      </c>
+      <c r="P22">
+        <v>11228.5926844924</v>
+      </c>
+      <c r="Q22">
+        <v>12664.5312011241</v>
+      </c>
+      <c r="R22">
+        <v>13743.485821411001</v>
+      </c>
+      <c r="S22">
+        <v>14350.6542555987</v>
+      </c>
+      <c r="T22">
+        <v>15551.9964639097</v>
+      </c>
+      <c r="U22">
+        <v>21449.238313361999</v>
+      </c>
+      <c r="V22">
+        <v>26489.108288660598</v>
+      </c>
+      <c r="W22">
+        <v>46903.2757859677</v>
+      </c>
+      <c r="X22">
+        <v>129889.292085543</v>
+      </c>
+      <c r="Y22">
+        <v>419716.14590473397</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>450184.25380215701</v>
+      </c>
+      <c r="C23">
+        <v>439537.68802810099</v>
+      </c>
+      <c r="D23">
+        <v>543050.79489411798</v>
+      </c>
+      <c r="E23">
+        <v>670000.59476766502</v>
+      </c>
+      <c r="F23">
+        <v>659351.021731916</v>
+      </c>
+      <c r="G23">
+        <v>884954.01192013803</v>
+      </c>
+      <c r="H23">
+        <v>1418719.79018991</v>
+      </c>
+      <c r="I23">
+        <v>936373.16030338802</v>
+      </c>
+      <c r="J23">
+        <v>1696464.6736341701</v>
+      </c>
+      <c r="K23">
+        <v>6004270.9108230304</v>
+      </c>
+      <c r="L23">
+        <v>14652419.9926401</v>
+      </c>
+      <c r="O23">
+        <v>8735.2316919714194</v>
+      </c>
+      <c r="P23">
+        <v>11342.577021569001</v>
+      </c>
+      <c r="Q23">
+        <v>12688.421936705699</v>
+      </c>
+      <c r="R23">
+        <v>13658.153947442701</v>
+      </c>
+      <c r="S23">
+        <v>14529.3767638504</v>
+      </c>
+      <c r="T23">
+        <v>15050.7364273071</v>
+      </c>
+      <c r="U23">
+        <v>21432.472098618699</v>
+      </c>
+      <c r="V23">
+        <v>26386.057676747401</v>
+      </c>
+      <c r="W23">
+        <v>46982.530264183799</v>
+      </c>
+      <c r="X23">
+        <v>129736.17026954801</v>
+      </c>
+      <c r="Y23">
+        <v>416948.37646745099</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>442699.01936745999</v>
+      </c>
+      <c r="C24">
+        <v>400612.82326824701</v>
+      </c>
+      <c r="D24">
+        <v>554151.71130634204</v>
+      </c>
+      <c r="E24">
+        <v>669233.78620558104</v>
+      </c>
+      <c r="F24">
+        <v>675150.80915966094</v>
+      </c>
+      <c r="G24">
+        <v>865224.005457622</v>
+      </c>
+      <c r="H24">
+        <v>1450403.2818329299</v>
+      </c>
+      <c r="I24">
+        <v>925821.02136516199</v>
+      </c>
+      <c r="J24">
+        <v>1733608.3113192599</v>
+      </c>
+      <c r="K24">
+        <v>5996150.5952707501</v>
+      </c>
+      <c r="L24">
+        <v>14588678.7631495</v>
+      </c>
+      <c r="O24">
+        <v>8750.6659757345897</v>
+      </c>
+      <c r="P24">
+        <v>11279.234528541499</v>
+      </c>
+      <c r="Q24">
+        <v>12667.613415047501</v>
+      </c>
+      <c r="R24">
+        <v>13763.026200234801</v>
+      </c>
+      <c r="S24">
+        <v>14776.608467102</v>
+      </c>
+      <c r="T24">
+        <v>15087.968196719799</v>
+      </c>
+      <c r="U24">
+        <v>21402.839474380002</v>
+      </c>
+      <c r="V24">
+        <v>26341.350927948901</v>
+      </c>
+      <c r="W24">
+        <v>46820.3050885349</v>
+      </c>
+      <c r="X24">
+        <v>130430.350769311</v>
+      </c>
+      <c r="Y24">
+        <v>417936.79221533198</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>443738.30427965801</v>
+      </c>
+      <c r="C25">
+        <v>444239.56713787001</v>
+      </c>
+      <c r="D25">
+        <v>573609.46217464295</v>
+      </c>
+      <c r="E25">
+        <v>661128.76748528401</v>
+      </c>
+      <c r="F25">
+        <v>673163.75734188606</v>
+      </c>
+      <c r="G25">
+        <v>863487.50474986201</v>
+      </c>
+      <c r="H25">
+        <v>1462662.7711853599</v>
+      </c>
+      <c r="I25">
+        <v>913443.21992350498</v>
+      </c>
+      <c r="J25">
+        <v>1714255.55192142</v>
+      </c>
+      <c r="K25">
+        <v>6050715.1808049399</v>
+      </c>
+      <c r="L25">
+        <v>14627096.303513501</v>
+      </c>
+      <c r="O25">
+        <v>8742.8540755063295</v>
+      </c>
+      <c r="P25">
+        <v>11295.3914664685</v>
+      </c>
+      <c r="Q25">
+        <v>12746.406763792</v>
+      </c>
+      <c r="R25">
+        <v>13710.479307919701</v>
+      </c>
+      <c r="S25">
+        <v>14864.016957581</v>
+      </c>
+      <c r="T25">
+        <v>15078.9930112659</v>
+      </c>
+      <c r="U25">
+        <v>21487.774129956899</v>
+      </c>
+      <c r="V25">
+        <v>26463.1190355867</v>
+      </c>
+      <c r="W25">
+        <v>46898.2236310839</v>
+      </c>
+      <c r="X25">
+        <v>129164.245016872</v>
+      </c>
+      <c r="Y25">
+        <v>421718.94021890999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>457764.667560993</v>
+      </c>
+      <c r="C26">
+        <v>425392.856830089</v>
+      </c>
+      <c r="D26">
+        <v>557221.77865784802</v>
+      </c>
+      <c r="E26">
+        <v>670958.660737328</v>
+      </c>
+      <c r="F26">
+        <v>679189.88290436997</v>
+      </c>
+      <c r="G26">
+        <v>880835.87174135097</v>
+      </c>
+      <c r="H26">
+        <v>1467021.61452887</v>
+      </c>
+      <c r="I26">
+        <v>941855.83488003805</v>
+      </c>
+      <c r="J26">
+        <v>1718786.4889275499</v>
+      </c>
+      <c r="K26">
+        <v>6028133.4769543102</v>
+      </c>
+      <c r="L26">
+        <v>14647109.186931901</v>
+      </c>
+      <c r="O26">
+        <v>8735.7209958136009</v>
+      </c>
+      <c r="P26">
+        <v>11345.712447538899</v>
+      </c>
+      <c r="Q26">
+        <v>12789.283905178299</v>
+      </c>
+      <c r="R26">
+        <v>13679.760305210901</v>
+      </c>
+      <c r="S26">
+        <v>14727.4562679231</v>
+      </c>
+      <c r="T26">
+        <v>15040.159927680999</v>
+      </c>
+      <c r="U26">
+        <v>21429.887272417502</v>
+      </c>
+      <c r="V26">
+        <v>26434.605209156802</v>
+      </c>
+      <c r="W26">
+        <v>46722.871776670203</v>
+      </c>
+      <c r="X26">
+        <v>129578.92547734</v>
+      </c>
+      <c r="Y26">
+        <v>422872.26403504598</v>
+      </c>
+    </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>AVERAGE(B17:B26)</f>
-        <v>446422.21549704333</v>
+        <v>447633.79583911027</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27" si="12">AVERAGE(C17:C26)</f>
-        <v>423718.28504918178</v>
+        <v>426495.3841927062</v>
       </c>
       <c r="D27">
         <f t="shared" ref="D27" si="13">AVERAGE(D17:D26)</f>
-        <v>557058.91362792754</v>
+        <v>558572.35844322201</v>
       </c>
       <c r="E27">
         <f t="shared" ref="E27" si="14">AVERAGE(E17:E26)</f>
-        <v>678546.44492490438</v>
+        <v>671952.66624934785</v>
       </c>
       <c r="F27">
         <f t="shared" ref="F27" si="15">AVERAGE(F17:F26)</f>
-        <v>672164.72672359971</v>
+        <v>673518.00051370065</v>
       </c>
       <c r="G27">
         <f t="shared" ref="G27" si="16">AVERAGE(G17:G26)</f>
-        <v>869045.76879791566</v>
+        <v>871416.85732310056</v>
       </c>
       <c r="H27">
         <f t="shared" ref="H27" si="17">AVERAGE(H17:H26)</f>
-        <v>1452984.68745348</v>
+        <v>1451640.2628366561</v>
       </c>
       <c r="I27">
         <f t="shared" ref="I27" si="18">AVERAGE(I17:I26)</f>
-        <v>930698.06743964984</v>
+        <v>931916.13063252089</v>
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="19">AVERAGE(J17:J26)</f>
-        <v>1726782.1057293378</v>
+        <v>1721963.0816064938</v>
       </c>
       <c r="K27">
         <f t="shared" ref="K27" si="20">AVERAGE(K17:K26)</f>
-        <v>6033229.4937768634</v>
+        <v>6025242.1700546201</v>
       </c>
       <c r="L27">
         <f t="shared" ref="L27" si="21">AVERAGE(L17:L26)</f>
-        <v>14610840.15491778</v>
+        <v>14615843.580671091</v>
       </c>
       <c r="O27">
         <f>AVERAGE(O17:O26)</f>
-        <v>9495.7179058343118</v>
+        <v>9127.292271703478</v>
       </c>
       <c r="P27">
         <f t="shared" ref="P27" si="22">AVERAGE(P17:P26)</f>
-        <v>12574.18142706152</v>
+        <v>11936.241528391789</v>
       </c>
       <c r="Q27">
         <f t="shared" ref="Q27" si="23">AVERAGE(Q17:Q26)</f>
-        <v>14280.234437063298</v>
+        <v>13495.742940716407</v>
       </c>
       <c r="R27">
         <f t="shared" ref="R27" si="24">AVERAGE(R17:R26)</f>
-        <v>15604.71945442256</v>
+        <v>14657.850285433189</v>
       </c>
       <c r="S27">
         <f t="shared" ref="S27" si="25">AVERAGE(S17:S26)</f>
-        <v>16458.980408310839</v>
+        <v>15554.301475360935</v>
       </c>
       <c r="T27">
         <f t="shared" ref="T27" si="26">AVERAGE(T17:T26)</f>
-        <v>17176.501053571661</v>
+        <v>16169.235929474182</v>
       </c>
       <c r="U27">
         <f t="shared" ref="U27" si="27">AVERAGE(U17:U26)</f>
-        <v>26877.040414139599</v>
+        <v>24158.741335943305</v>
       </c>
       <c r="V27">
         <f t="shared" ref="V27" si="28">AVERAGE(V17:V26)</f>
-        <v>32792.380711436221</v>
+        <v>29607.614469528151</v>
       </c>
       <c r="W27">
         <f t="shared" ref="W27" si="29">AVERAGE(W17:W26)</f>
-        <v>60130.045841261686</v>
+        <v>53497.743575274901</v>
       </c>
       <c r="X27">
         <f t="shared" ref="X27" si="30">AVERAGE(X17:X26)</f>
-        <v>157293.32219883738</v>
+        <v>143526.55946128009</v>
       </c>
       <c r="Y27">
         <f t="shared" ref="Y27" si="31">AVERAGE(Y17:Y26)</f>
-        <v>464966.60928130103</v>
+        <v>442402.55652479781</v>
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
@@ -1560,47 +2240,47 @@
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29">
         <f>B27/B28</f>
-        <v>4.1274624903803039</v>
+        <v>4.1386643352759389</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:L29" si="32">C27/C28</f>
-        <v>9.5640991591806834</v>
+        <v>9.6267833824505384</v>
       </c>
       <c r="D29">
         <f t="shared" si="32"/>
-        <v>9.4368780895803415</v>
+        <v>9.46251666005797</v>
       </c>
       <c r="E29">
         <f t="shared" si="32"/>
-        <v>7.0118055318160666</v>
+        <v>6.9436682743908138</v>
       </c>
       <c r="F29">
         <f t="shared" si="32"/>
-        <v>11.482732745504547</v>
+        <v>11.505851008997739</v>
       </c>
       <c r="G29">
         <f t="shared" si="32"/>
-        <v>11.79454641293553</v>
+        <v>11.826726436892329</v>
       </c>
       <c r="H29">
         <f t="shared" si="32"/>
-        <v>18.078919576621335</v>
+        <v>18.062191427498863</v>
       </c>
       <c r="I29">
         <f t="shared" si="32"/>
-        <v>18.941651927132387</v>
+        <v>18.966442060293495</v>
       </c>
       <c r="J29">
         <f t="shared" si="32"/>
-        <v>16.105487989118682</v>
+        <v>16.060541533586033</v>
       </c>
       <c r="K29">
         <f t="shared" si="32"/>
-        <v>23.290275796779955</v>
+        <v>23.259442066261151</v>
       </c>
       <c r="L29">
         <f t="shared" si="32"/>
-        <v>38.649744346821912</v>
+        <v>38.662979802427017</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C547523A-001A-429F-83FC-D387C3E4E712}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>

</xml_diff>